<commit_message>
change feat> These files will always undergo changes as they are files that will receive inputs - they will always be editable
</commit_message>
<xml_diff>
--- a/dados/base_pecas.xlsx
+++ b/dados/base_pecas.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\usuario\statistical-project\dados\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64335E5-1A86-40BD-95DC-10316E9B91CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ID</t>
   </si>
@@ -38,12 +44,6 @@
   </si>
   <si>
     <t>SUPORTE DO CHICOTE DO MOTOR</t>
-  </si>
-  <si>
-    <t>46357616</t>
-  </si>
-  <si>
-    <t>5980</t>
   </si>
   <si>
     <t>dados/peca_1/txt</t>
@@ -55,11 +55,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,13 +123,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -167,7 +175,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -201,6 +209,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -235,9 +244,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -410,14 +420,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="6" max="6" width="22" customWidth="1"/>
+    <col min="7" max="7" width="9.77734375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,28 +460,31 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>46357616</v>
+      </c>
+      <c r="D2">
+        <v>5980</v>
+      </c>
+      <c r="E2" s="2">
+        <v>45955.717697916669</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2">
-        <v>45955.71769791361</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add files from imputs
</commit_message>
<xml_diff>
--- a/dados/base_pecas.xlsx
+++ b/dados/base_pecas.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\usuario\statistical-project\dados\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64335E5-1A86-40BD-95DC-10316E9B91CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -46,7 +40,25 @@
     <t>SUPORTE DO CHICOTE DO MOTOR</t>
   </si>
   <si>
+    <t>crossmember</t>
+  </si>
+  <si>
+    <t>chifre</t>
+  </si>
+  <si>
+    <t>53489571</t>
+  </si>
+  <si>
+    <t>5980</t>
+  </si>
+  <si>
     <t>dados/peca_1/txt</t>
+  </si>
+  <si>
+    <t>dados/peca_2/txt</t>
+  </si>
+  <si>
+    <t>dados/peca_3/txt</t>
   </si>
   <si>
     <t>Ativa</t>
@@ -55,11 +67,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,21 +135,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -175,7 +179,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -209,7 +213,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -244,10 +247,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -420,24 +422,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="9.77734375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -460,7 +452,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -474,17 +466,60 @@
         <v>5980</v>
       </c>
       <c r="E2" s="2">
-        <v>45955.717697916669</v>
+        <v>45955.71769791667</v>
       </c>
       <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="C3">
+        <v>53489514</v>
+      </c>
+      <c r="D3">
+        <v>5980</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45957.62032447917</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E3" s="2"/>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2">
+        <v>45957.62969117925</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add feature: I finalized the page that calculates conformity per piece - I created the page that calculates the cp and cpk per piece.
</commit_message>
<xml_diff>
--- a/dados/base_pecas.xlsx
+++ b/dados/base_pecas.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -570,25 +570,54 @@
           <t>staffa</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>53495349</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="C5" t="n">
+        <v>53495349</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5980</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>45960.63015388889</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>dados/peca_4/txt</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Ativa</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>LONGUERONE CPL LT</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>53489572</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>5980</t>
         </is>
       </c>
-      <c r="E5" s="2" t="n">
-        <v>45960.63015389245</v>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>dados/peca_4/txt</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
+      <c r="E6" s="2" t="n">
+        <v>45969.89631894375</v>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>dados/peca_5/txt</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>Ativa</t>
         </is>

</xml_diff>